<commit_message>
3.0.14 Fix a bug when the handling POI Excel Cell is null. Allow Test skipped.
Signed-off-by: Sinri Edogawa <ljni@leqee.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/excel_1.xlsx
+++ b/src/test/resources/excel/excel_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leqee/code/Keel/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A1DA59-DB61-724D-8961-A6325E573986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1531B0D1-0EA7-BF40-9D72-D871FE7EF588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="500" windowWidth="28020" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5295" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5294" uniqueCount="16">
   <si>
     <t>record_id</t>
   </si>
@@ -598,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1764"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1738" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F1764"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
@@ -720,9 +720,6 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
       <c r="F6">
         <v>1.5</v>
       </c>

</xml_diff>